<commit_message>
feat: teach make how to find dependencies
This adds a "pending" column to the database, which indicates whether or
not a reagent has been synthesized yet.  By default, `sw make` will
automatically find and include any pending dependencies in its protocol.
</commit_message>
<xml_diff>
--- a/tests/mock_excel_db/fragments.xlsx
+++ b/tests/mock_excel_db/fragments.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -62,6 +62,9 @@
     <t xml:space="preserve">Circular</t>
   </si>
   <si>
+    <t xml:space="preserve">Pending</t>
+  </si>
+  <si>
     <t xml:space="preserve">f2</t>
   </si>
   <si>
@@ -174,6 +177,12 @@
   </si>
   <si>
     <t xml:space="preserve">mock circular=y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pending from db</t>
   </si>
 </sst>
 </file>
@@ -280,15 +289,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+      <selection pane="bottomLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.2"/>
@@ -338,57 +347,60 @@
       <c r="L1" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>44305</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H6" s="2" t="n">
         <v>5000</v>
@@ -396,68 +408,68 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K12" s="0" t="n">
         <v>10</v>
@@ -465,35 +477,46 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="M16" s="0" t="s">
         <v>47</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: rename the 'pending' column to 'ready'
</commit_message>
<xml_diff>
--- a/tests/mock_excel_db/fragments.xlsx
+++ b/tests/mock_excel_db/fragments.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -62,7 +62,7 @@
     <t xml:space="preserve">Circular</t>
   </si>
   <si>
-    <t xml:space="preserve">Pending</t>
+    <t xml:space="preserve">Ready</t>
   </si>
   <si>
     <t xml:space="preserve">f2</t>
@@ -182,7 +182,10 @@
     <t xml:space="preserve">f16</t>
   </si>
   <si>
-    <t xml:space="preserve">pending from db</t>
+    <t xml:space="preserve">ready from db</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n</t>
   </si>
 </sst>
 </file>
@@ -294,10 +297,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+      <selection pane="bottomLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.2"/>
@@ -516,7 +519,7 @@
         <v>52</v>
       </c>
       <c r="M16" s="0" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>